<commit_message>
Changes in Test Data.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15690" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15690" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:I18"/>
+  <oleSize ref="A1:K18"/>
 </workbook>
 </file>
 
@@ -68,9 +68,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Positive</t>
-  </si>
-  <si>
     <t>FriendListTest</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Test Test</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -500,7 +500,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -533,10 +533,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>14</v>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -578,16 +578,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -630,13 +630,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>